<commit_message>
Ajout des TI du weekend
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_03_21.xlsx
+++ b/Excel/TI/Mon_TI_2024_03_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,12 +628,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>De'Aaron Fox</t>
+          <t>Damian Lillard</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -648,85 +648,83 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>34</v>
+        <v>40.8</v>
       </c>
       <c r="G2" t="n">
-        <v>37.3</v>
+        <v>35</v>
       </c>
       <c r="H2" t="n">
-        <v>36</v>
+        <v>35.6</v>
       </c>
       <c r="I2" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N2" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="O2" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="P2" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="n">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="R2" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1.2</v>
+        <v>1.9</v>
       </c>
       <c r="U2" t="n">
-        <v>-6.3</v>
+        <v>-1.4</v>
       </c>
       <c r="V2" t="n">
+        <v>9</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z2" t="n">
         <v>11</v>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z2" t="n">
-        <v>46</v>
-      </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
+        <v>33</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
@@ -740,12 +738,12 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -755,27 +753,27 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>ATL</t>
         </is>
       </c>
     </row>
@@ -802,16 +800,16 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>33.4</v>
+        <v>34.2</v>
       </c>
       <c r="G3" t="n">
-        <v>34.9</v>
+        <v>35</v>
       </c>
       <c r="H3" t="n">
-        <v>40.8</v>
+        <v>40.7</v>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -820,38 +818,36 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M3" t="n">
         <v>2</v>
       </c>
       <c r="N3" t="n">
+        <v>36</v>
+      </c>
+      <c r="O3" t="n">
         <v>33</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>34</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>30</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>38</v>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="S3" t="inlineStr">
         <is>
           <t>vs</t>
         </is>
       </c>
       <c r="T3" t="n">
-        <v>-1.6</v>
+        <v>-1.7</v>
       </c>
       <c r="U3" t="n">
-        <v>-12.5</v>
+        <v>-12.4</v>
       </c>
       <c r="V3" t="n">
         <v>9</v>
@@ -938,12 +934,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Damian Lillard</t>
+          <t>Dejounte Murray</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -952,89 +948,83 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>39.6</v>
+        <v>33.4</v>
       </c>
       <c r="G4" t="n">
         <v>33.5</v>
       </c>
       <c r="H4" t="n">
-        <v>35.4</v>
+        <v>31.5</v>
       </c>
       <c r="I4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
       </c>
       <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
         <v>3</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
       </c>
       <c r="M4" t="n">
         <v>6</v>
       </c>
       <c r="N4" t="n">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="O4" t="n">
+        <v>33</v>
+      </c>
+      <c r="P4" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>48</v>
+      </c>
+      <c r="R4" t="n">
         <v>27</v>
       </c>
-      <c r="P4" t="n">
-        <v>13</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>60</v>
-      </c>
-      <c r="R4" t="n">
-        <v>41</v>
-      </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="U4" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="V4" t="n">
-        <v>9</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AB4" t="n">
-        <v>33</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
@@ -1053,7 +1043,7 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
@@ -1063,39 +1053,39 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dejounte Murray</t>
+          <t>Bradley Beal</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1104,18 +1094,22 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F5" t="n">
-        <v>33.4</v>
+        <v>30.6</v>
       </c>
       <c r="G5" t="n">
-        <v>33.5</v>
+        <v>31.7</v>
       </c>
       <c r="H5" t="n">
-        <v>31.5</v>
+        <v>27</v>
       </c>
       <c r="I5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J5" t="n">
         <v>2</v>
@@ -1124,53 +1118,57 @@
         <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O5" t="n">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="P5" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="Q5" t="n">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="R5" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
+        <v>-1.6</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="V5" t="n">
+        <v>7</v>
+      </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
@@ -1194,105 +1192,101 @@
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>OKC</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bradley Beal</t>
+          <t>Michael Porter Jr.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>14</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" t="n">
+        <v>35</v>
+      </c>
+      <c r="O6" t="n">
+        <v>35</v>
+      </c>
+      <c r="P6" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q6" t="n">
         <v>36</v>
       </c>
-      <c r="G6" t="n">
-        <v>32.1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>27.4</v>
-      </c>
-      <c r="I6" t="n">
-        <v>9</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" t="n">
-        <v>4</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>48</v>
-      </c>
-      <c r="O6" t="n">
-        <v>28</v>
-      </c>
-      <c r="P6" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>35</v>
-      </c>
       <c r="R6" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1300,14 +1294,10 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="U6" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="V6" t="n">
-        <v>7</v>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr">
         <is>
           <t>vs</t>
@@ -1315,7 +1305,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1324,7 +1314,7 @@
         </is>
       </c>
       <c r="Z6" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -1353,124 +1343,124 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>MIN</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Michael Porter Jr.</t>
+          <t>Nikola Vucevic</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>32.2</v>
+        <v>30.2</v>
       </c>
       <c r="G7" t="n">
         <v>30.8</v>
       </c>
       <c r="H7" t="n">
-        <v>24.6</v>
+        <v>30.6</v>
       </c>
       <c r="I7" t="n">
         <v>14</v>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N7" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="O7" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="P7" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="Q7" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="R7" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="Z7" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1494,12 +1484,12 @@
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
@@ -1509,7 +1499,7 @@
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
@@ -1519,76 +1509,92 @@
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>BKN</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nikola Vucevic</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>Lauri Markkanen</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Day-To-Day</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F8" t="n">
-        <v>30.2</v>
+        <v>28.8</v>
       </c>
       <c r="G8" t="n">
-        <v>30.8</v>
+        <v>29.3</v>
       </c>
       <c r="H8" t="n">
-        <v>30.6</v>
+        <v>35</v>
       </c>
       <c r="I8" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>2</v>
-      </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" t="n">
-        <v>8</v>
       </c>
       <c r="M8" t="n">
         <v>2</v>
       </c>
-      <c r="N8" t="n">
-        <v>32</v>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="O8" t="n">
-        <v>50</v>
-      </c>
-      <c r="P8" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>21</v>
-      </c>
-      <c r="R8" t="n">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1596,10 +1602,14 @@
         </is>
       </c>
       <c r="T8" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
+        <v>-2.6</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="V8" t="n">
+        <v>7</v>
+      </c>
       <c r="W8" t="inlineStr">
         <is>
           <t>@</t>
@@ -1607,47 +1617,47 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z8" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
           <t>HOU</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z8" t="n">
-        <v>33</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>BOS</t>
-        </is>
-      </c>
       <c r="AG8" t="inlineStr">
         <is>
           <t>vs</t>
@@ -1655,7 +1665,7 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
@@ -1665,17 +1675,17 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>HOU</t>
         </is>
       </c>
     </row>
@@ -1980,7 +1990,11 @@
           <t>Nic Claxton</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>C</t>
@@ -2140,16 +2154,16 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>25</v>
+        <v>28.8</v>
       </c>
       <c r="G12" t="n">
-        <v>24.7</v>
+        <v>25.9</v>
       </c>
       <c r="H12" t="n">
-        <v>23.6</v>
+        <v>24</v>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -2161,16 +2175,14 @@
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
+        <v>41</v>
+      </c>
+      <c r="O12" t="n">
         <v>36</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="P12" t="inlineStr">
         <is>
           <t>-</t>
@@ -2192,10 +2204,10 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.6</v>
+        <v>-1</v>
       </c>
       <c r="V12" t="n">
         <v>1</v>
@@ -2884,172 +2896,6 @@
       <c r="AL16" t="inlineStr">
         <is>
           <t>DET</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>UTA</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Lauri Markkanen</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>28.8</v>
-      </c>
-      <c r="G17" t="n">
-        <v>29.3</v>
-      </c>
-      <c r="H17" t="n">
-        <v>35</v>
-      </c>
-      <c r="I17" t="n">
-        <v>6</v>
-      </c>
-      <c r="J17" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" t="n">
-        <v>2</v>
-      </c>
-      <c r="M17" t="n">
-        <v>2</v>
-      </c>
-      <c r="N17" t="n">
-        <v>34</v>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="T17" t="n">
-        <v>-2.6</v>
-      </c>
-      <c r="U17" t="n">
-        <v>-1</v>
-      </c>
-      <c r="V17" t="n">
-        <v>7</v>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z17" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE17" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF17" t="inlineStr">
-        <is>
-          <t>HOU</t>
-        </is>
-      </c>
-      <c r="AG17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH17" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="AI17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AJ17" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="AK17" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AL17" t="inlineStr">
-        <is>
-          <t>HOU</t>
         </is>
       </c>
     </row>

</xml_diff>